<commit_message>
Cleaned up all the page object (i.e. locator names, filename convention to include page_object) and test data files (remove unneeded files)
</commit_message>
<xml_diff>
--- a/selenium_tests/lti_emailer/test_data/roles_access.xlsx
+++ b/selenium_tests/lti_emailer/test_data/roles_access.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3320" yWindow="-18460" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="testing_access" sheetId="1" r:id="rId1"/>
     <sheet name="Roles mapping " sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="46">
   <si>
     <t xml:space="preserve">denied_roles </t>
   </si>
@@ -164,7 +165,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -187,11 +188,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
     </font>
     <font>
       <sz val="12"/>
@@ -239,7 +235,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="130">
+  <cellStyleXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -370,21 +366,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="129"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="129"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="130">
+  <cellStyles count="138">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -449,6 +452,14 @@
     <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -843,20 +854,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B7" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="17" style="2" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="2"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -864,7 +870,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -872,7 +878,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -880,7 +886,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -888,7 +894,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -896,7 +902,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -904,7 +910,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -912,7 +918,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -920,7 +926,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
         <v>26</v>
       </c>
@@ -928,7 +934,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
@@ -936,7 +942,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
         <v>28</v>
       </c>
@@ -944,7 +950,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
         <v>29</v>
       </c>
@@ -952,26 +958,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="N13" s="3"/>
-    </row>
-    <row r="14" spans="1:14">
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="N14" s="1"/>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="N15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1001,13 +1002,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -1015,13 +1016,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="20">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>79592</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -1029,13 +1030,13 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="20">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>79593</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -1043,13 +1044,13 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="20">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>79588</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -1057,13 +1058,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="20">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>79589</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -1071,13 +1072,13 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="20">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>79557</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -1085,13 +1086,13 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="20">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>79505</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -1099,79 +1100,79 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="20">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <v>79494</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="20">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>79594</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="20">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <v>79584</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="20">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>79585</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="20">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <v>79577</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="20">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <v>79610</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="20">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <v>79611</v>
       </c>
     </row>
@@ -1193,4 +1194,137 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix broken tests to use new canvas dev instance and clean up code
</commit_message>
<xml_diff>
--- a/selenium_tests/lti_emailer/test_data/roles_access.xlsx
+++ b/selenium_tests/lti_emailer/test_data/roles_access.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="testing_access" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="52">
   <si>
     <t xml:space="preserve">denied_roles </t>
   </si>
@@ -159,6 +159,24 @@
   </si>
   <si>
     <t>79611</t>
+  </si>
+  <si>
+    <t>92241</t>
+  </si>
+  <si>
+    <t>92242</t>
+  </si>
+  <si>
+    <t>92229</t>
+  </si>
+  <si>
+    <t>92230</t>
+  </si>
+  <si>
+    <t>92232</t>
+  </si>
+  <si>
+    <t>92258</t>
   </si>
 </sst>
 </file>
@@ -375,7 +393,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -386,6 +404,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="138">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -857,10 +876,14 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="A1:XFD1048576"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
@@ -919,40 +942,40 @@
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="2" t="s">
-        <v>25</v>
+      <c r="A8" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="2" t="s">
-        <v>26</v>
+      <c r="A9" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="2" t="s">
-        <v>27</v>
+      <c r="A10" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="2" t="s">
-        <v>28</v>
+      <c r="A11" s="8" t="s">
+        <v>49</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="2" t="s">
-        <v>29</v>
+      <c r="A12" s="8" t="s">
+        <v>50</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>24</v>
@@ -967,8 +990,8 @@
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="2" t="s">
-        <v>45</v>
+      <c r="A14" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>24</v>
@@ -989,8 +1012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1109,6 +1132,9 @@
       <c r="C8" s="6">
         <v>79494</v>
       </c>
+      <c r="D8">
+        <v>92241</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="20">
       <c r="A9" s="7" t="s">
@@ -1120,6 +1146,9 @@
       <c r="C9" s="6">
         <v>79594</v>
       </c>
+      <c r="D9">
+        <v>92242</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="20">
       <c r="A10" s="7" t="s">
@@ -1131,6 +1160,9 @@
       <c r="C10" s="6">
         <v>79584</v>
       </c>
+      <c r="D10">
+        <v>92229</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="20">
       <c r="A11" s="7" t="s">
@@ -1142,6 +1174,9 @@
       <c r="C11" s="6">
         <v>79585</v>
       </c>
+      <c r="D11">
+        <v>92230</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="20">
       <c r="A12" s="7" t="s">
@@ -1153,6 +1188,9 @@
       <c r="C12" s="6">
         <v>79577</v>
       </c>
+      <c r="D12">
+        <v>92232</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="20">
       <c r="A13" s="7" t="s">
@@ -1164,6 +1202,9 @@
       <c r="C13" s="6">
         <v>79610</v>
       </c>
+      <c r="D13">
+        <v>92257</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="20">
       <c r="A14" s="7" t="s">
@@ -1174,6 +1215,9 @@
       </c>
       <c r="C14" s="6">
         <v>79611</v>
+      </c>
+      <c r="D14">
+        <v>92258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- updated locator element and added in a wait for the unauthorized message. - updated test data to reflect masquerade user ID.  some of the IDs used for the canvas.icommons instance (now deprecated) so it is now pointing to users who aren't the intended test ID in the course.
</commit_message>
<xml_diff>
--- a/selenium_tests/lti_emailer/test_data/roles_access.xlsx
+++ b/selenium_tests/lti_emailer/test_data/roles_access.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14760" tabRatio="500"/>
+    <workbookView xWindow="-15260" yWindow="-22740" windowWidth="25600" windowHeight="14380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="testing_access" sheetId="1" r:id="rId1"/>
@@ -21,74 +21,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="44">
   <si>
     <t xml:space="preserve">denied_roles </t>
   </si>
   <si>
-    <t>79592</t>
-  </si>
-  <si>
-    <t>79593</t>
-  </si>
-  <si>
-    <t>79588</t>
-  </si>
-  <si>
-    <t>79589</t>
-  </si>
-  <si>
-    <t>78557</t>
-  </si>
-  <si>
-    <t>79505</t>
-  </si>
-  <si>
     <t xml:space="preserve">Roles </t>
   </si>
   <si>
-    <t xml:space="preserve">ID </t>
-  </si>
-  <si>
     <t xml:space="preserve">Masquerade ID </t>
   </si>
   <si>
-    <t>Shopper</t>
-  </si>
-  <si>
-    <t>test13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Student </t>
-  </si>
-  <si>
-    <t>test14</t>
-  </si>
-  <si>
     <t xml:space="preserve">Guest </t>
   </si>
   <si>
-    <t>test7</t>
-  </si>
-  <si>
     <t>Harvard-Viewer</t>
   </si>
   <si>
-    <t>test8</t>
-  </si>
-  <si>
     <t>Observer</t>
   </si>
   <si>
-    <t>test11</t>
-  </si>
-  <si>
-    <t>SapnaRole</t>
-  </si>
-  <si>
-    <t>test77</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -98,24 +50,6 @@
     <t>yes</t>
   </si>
   <si>
-    <t>79494</t>
-  </si>
-  <si>
-    <t>79594</t>
-  </si>
-  <si>
-    <t>79584</t>
-  </si>
-  <si>
-    <t>79585</t>
-  </si>
-  <si>
-    <t>79577</t>
-  </si>
-  <si>
-    <t>79610</t>
-  </si>
-  <si>
     <t>test15@mcelroy.org</t>
   </si>
   <si>
@@ -131,12 +65,6 @@
     <t>test5@mcelroy.org</t>
   </si>
   <si>
-    <t>test33@mcelroy.org</t>
-  </si>
-  <si>
-    <t>test34@mcelroy.org</t>
-  </si>
-  <si>
     <t>TA</t>
   </si>
   <si>
@@ -152,15 +80,6 @@
     <t>Course Designer</t>
   </si>
   <si>
-    <t xml:space="preserve">Account admin (of subaccount 656) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">School Liaison (of subaccount 656) </t>
-  </si>
-  <si>
-    <t>79611</t>
-  </si>
-  <si>
     <t>92241</t>
   </si>
   <si>
@@ -176,7 +95,64 @@
     <t>92232</t>
   </si>
   <si>
-    <t>92258</t>
+    <t>92238</t>
+  </si>
+  <si>
+    <t>test11@mcelroy.org</t>
+  </si>
+  <si>
+    <t>92295</t>
+  </si>
+  <si>
+    <t>test80@mcelroy.org</t>
+  </si>
+  <si>
+    <t>tlttest54@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Access to Emailer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Course or Account Level Roles </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes </t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Course Level Role (course 27) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Account admin </t>
+  </si>
+  <si>
+    <t>School Liaison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Account Level Role (sub-account 10) </t>
+  </si>
+  <si>
+    <t>Account Level Role (sub-account 10)</t>
+  </si>
+  <si>
+    <t>test7@mcelroy.org</t>
+  </si>
+  <si>
+    <t>test8@mcelroy.org</t>
+  </si>
+  <si>
+    <t>92234</t>
+  </si>
+  <si>
+    <t>92235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90670 </t>
   </si>
 </sst>
 </file>
@@ -215,25 +191,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="15"/>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
-      <name val="Monaco"/>
+      <name val="Calibri"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
+      <sz val="16"/>
       <color theme="1"/>
-      <name val="Monaco"/>
+      <name val="Calibri"/>
     </font>
     <font>
-      <sz val="15"/>
-      <color theme="1"/>
-      <name val="Menlo Bold"/>
+      <sz val="16"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
     </font>
     <font>
-      <sz val="15"/>
-      <color rgb="FF808080"/>
-      <name val="Menlo"/>
+      <u/>
+      <sz val="16"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -253,7 +230,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="138">
+  <cellStyleXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -392,21 +369,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="129"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="129" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="138">
+  <cellStyles count="144">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -479,6 +461,12 @@
     <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -873,16 +861,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -890,111 +877,87 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="8" t="s">
-        <v>46</v>
-      </c>
       <c r="B8" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="8" t="s">
-        <v>47</v>
+      <c r="A9" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="8" t="s">
-        <v>48</v>
+      <c r="A10" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="8" t="s">
-        <v>49</v>
+      <c r="A11" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1010,225 +973,221 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" customWidth="1"/>
-    <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="50.33203125" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="39.1640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="31" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18" style="5" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="47.33203125" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20">
-      <c r="A1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="4" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="20">
-      <c r="A2" s="3" t="s">
+      <c r="C2" s="5">
+        <v>92241</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C3" s="5">
+        <v>92242</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3">
-        <v>79592</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="20">
-      <c r="A3" s="3" t="s">
+      <c r="C4" s="5">
+        <v>92229</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C5" s="5">
+        <v>92230</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="3">
-        <v>79593</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="20">
-      <c r="A4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="3">
-        <v>79588</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="C6" s="5">
+        <v>92232</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="5">
+        <v>92295</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="5">
+        <v>90670</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="20">
-      <c r="A5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="3">
-        <v>79589</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="B10" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="5">
+        <v>92234</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="20">
-      <c r="A6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="3">
-        <v>79557</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="B11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="5">
+        <v>92235</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="20">
-      <c r="A7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="3">
-        <v>79505</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="20">
-      <c r="A8" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="6">
-        <v>79494</v>
-      </c>
-      <c r="D8">
-        <v>92241</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="20">
-      <c r="A9" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="6">
-        <v>79594</v>
-      </c>
-      <c r="D9">
-        <v>92242</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="20">
-      <c r="A10" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="5" t="s">
+      <c r="B12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="5">
+        <v>92238</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="6">
-        <v>79584</v>
-      </c>
-      <c r="D10">
-        <v>92229</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="20">
-      <c r="A11" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="5" t="s">
+      <c r="E12" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="C11" s="6">
-        <v>79585</v>
-      </c>
-      <c r="D11">
-        <v>92230</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="20">
-      <c r="A12" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="6">
-        <v>79577</v>
-      </c>
-      <c r="D12">
-        <v>92232</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="20">
-      <c r="A13" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="6">
-        <v>79610</v>
-      </c>
-      <c r="D13">
-        <v>92257</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="20">
-      <c r="A14" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="6">
-        <v>79611</v>
-      </c>
-      <c r="D14">
-        <v>92258</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1"/>
-    <hyperlink ref="B9" r:id="rId2"/>
-    <hyperlink ref="B10" r:id="rId3"/>
-    <hyperlink ref="B11" r:id="rId4"/>
-    <hyperlink ref="B12" r:id="rId5"/>
-    <hyperlink ref="B13" r:id="rId6"/>
-    <hyperlink ref="B14" r:id="rId7"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="B8" r:id="rId7"/>
+    <hyperlink ref="B10" r:id="rId8"/>
+    <hyperlink ref="B11" r:id="rId9"/>
+    <hyperlink ref="B12" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1242,124 +1201,103 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D14" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="B8" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="2" t="s">
-        <v>26</v>
+      <c r="A9" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="2" t="s">
-        <v>28</v>
+      <c r="A11" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>